<commit_message>
working on testng param to get testcase run while true
</commit_message>
<xml_diff>
--- a/automation/src/main/resources/TestData/TestData.xlsx
+++ b/automation/src/main/resources/TestData/TestData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NAM\FPT Academy\AutoTestWeb\Selenium_automation\automation\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A89891AA-8B2F-4BBE-B1C5-BEC65B3EB9D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC65C62-BA53-469F-8648-40B0DFF9249D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9072" xr2:uid="{724AD072-28AB-42D3-B93E-091CFC78A356}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TestCase</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>Le</t>
+  </si>
+  <si>
+    <t>tc2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le </t>
+  </si>
+  <si>
+    <t>Hoang</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -98,8 +116,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF46DFEB-E095-4007-AFE8-A5CB34A2FEA2}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,8 +486,8 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="b">
-        <v>1</v>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -478,6 +497,23 @@
       </c>
       <c r="E2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>